<commit_message>
SRS Ordner erstellt Content Analyse erweitert
</commit_message>
<xml_diff>
--- a/Content Analyse.xlsx
+++ b/Content Analyse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabian\workspace\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabi\workspace\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="365">
   <si>
     <t>Content Analyse RZ-Webseite</t>
   </si>
@@ -641,9 +641,6 @@
     <t>Slider, Einkauf, Reparatur, Ausleihe</t>
   </si>
   <si>
-    <t>allg. Info</t>
-  </si>
-  <si>
     <t>Dienste d. RZ, Allgemeines</t>
   </si>
   <si>
@@ -711,6 +708,417 @@
   </si>
   <si>
     <t>Kontaktdaten Support, Schulungsangebot</t>
+  </si>
+  <si>
+    <t>Information zu Drucken, FAQ</t>
+  </si>
+  <si>
+    <t>Information zu Druck im CIP-Pool, Support</t>
+  </si>
+  <si>
+    <t>detaillierte Info zu Kosten / Einstellungen und Programmen d. Posterdrucks, Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information zu Email / Groupwise / Programmen, FAQ </t>
+  </si>
+  <si>
+    <t>Einrichtung von Apple Mail, Support</t>
+  </si>
+  <si>
+    <t>Einrichtung von Outlook, Support</t>
+  </si>
+  <si>
+    <t>Einrichtung von Thunderbird, Support</t>
+  </si>
+  <si>
+    <t>Verlinkung zu Webmail, Support</t>
+  </si>
+  <si>
+    <t>FAQs mit Tagsystem (5 Seiten)</t>
+  </si>
+  <si>
+    <t>Formulare verschiedener Kategorien</t>
+  </si>
+  <si>
+    <t>allgemeine Information zum Infostand, Öffnungszeiten, FAQs</t>
+  </si>
+  <si>
+    <t>Auflistung des Serviceangebots</t>
+  </si>
+  <si>
+    <t>Angebotene Produkte des Shops</t>
+  </si>
+  <si>
+    <t>Geschichte und Mitarbeiter d. Infostands</t>
+  </si>
+  <si>
+    <t>Informationen zu Wohnheim-Internet, Registrierung, An-/Abmeldung, Schritt f. Schritt Anleitung, FAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informationen zu Leistung und Einschränkungen, Formulare </t>
+  </si>
+  <si>
+    <t>allg. Informationen und Anleitungen</t>
+  </si>
+  <si>
+    <t>Informationen und Support (Windows und Mac)</t>
+  </si>
+  <si>
+    <t>Browserzugriff Netstorage Info, Support</t>
+  </si>
+  <si>
+    <t>Installation Novell, Support</t>
+  </si>
+  <si>
+    <t>Installation WebDAV, Support (Windows und Mac)</t>
+  </si>
+  <si>
+    <t>versch. Möglichkeiten Passwort zu erneuern</t>
+  </si>
+  <si>
+    <t>Informationen zur Synchronisation, Registrierung und Konfiguration</t>
+  </si>
+  <si>
+    <t>Anleitung Einrichten der Synchronisation über Android</t>
+  </si>
+  <si>
+    <t>Anleitung Einrichten der Synchronisation über Blackberry</t>
+  </si>
+  <si>
+    <t>Anleitung Einrichten der Synchronisation über iPhone/iOS</t>
+  </si>
+  <si>
+    <t>Links zu Softwareangeboten, FAQ</t>
+  </si>
+  <si>
+    <t>Link zu Citavi-Download, Support</t>
+  </si>
+  <si>
+    <t>Anleitung zu DreamSpark und dessen Nutzung</t>
+  </si>
+  <si>
+    <t>Info zu Installation und Umgang von SPSS, Support</t>
+  </si>
+  <si>
+    <t>Erklärung und Info zu VPN, FAQ</t>
+  </si>
+  <si>
+    <t>Installation und Nutzung von Juniper unter iOS, Hinweise</t>
+  </si>
+  <si>
+    <t>Installation und Nutzung von Juniper unter Mac OS</t>
+  </si>
+  <si>
+    <t>Installation und Nutzung von Juniper unter Windows Hinweise</t>
+  </si>
+  <si>
+    <t>Info Nutzung WLAN unter versch. Betriebssystemen, FAQ, Sicherheitshinweis Android</t>
+  </si>
+  <si>
+    <t>Beschreibung und Verlinkung</t>
+  </si>
+  <si>
+    <t>Konfigurationsanleitung, Support</t>
+  </si>
+  <si>
+    <t>Konfigurationsanleitung</t>
+  </si>
+  <si>
+    <t>Beschreibung und Information zu Workgroupmanagern, weiterführende Links, FAQ</t>
+  </si>
+  <si>
+    <t>Auflistung Workgroupmanager</t>
+  </si>
+  <si>
+    <t>SW-Bestellung, Angebot, Lizenzbedingungen, Campus Agreement, Übersicht Kauf-Lizenzen</t>
+  </si>
+  <si>
+    <t>Windows f. Studierende / Mitarbeiter, Ende Support Win XP Hinweis</t>
+  </si>
+  <si>
+    <t>externer Link (diverse Software)</t>
+  </si>
+  <si>
+    <t>Übersicht ReX, Dateimigration Info</t>
+  </si>
+  <si>
+    <t>Allgemeine Information ReX</t>
+  </si>
+  <si>
+    <t>Info Login, Laufwerke, Email, Kommandos, NCP-Server</t>
+  </si>
+  <si>
+    <t>Softwareangebot, Standard-Software, VPN, Dokumentation</t>
+  </si>
+  <si>
+    <t>Infomrationen Backup, Anleitungen Backup</t>
+  </si>
+  <si>
+    <t>Anleitung Drucken, Architektur, Administration, iPrint-Integration</t>
+  </si>
+  <si>
+    <t>Information zu Nutzung von Live-Linux</t>
+  </si>
+  <si>
+    <t>Migration der Linux-Homeverzeichnisse auf neues Fileserver-Cluster</t>
+  </si>
+  <si>
+    <t>externer Link (Uni-interne MsOffice-Seiten)</t>
+  </si>
+  <si>
+    <t>Information über SW-Angebot f. Studenten</t>
+  </si>
+  <si>
+    <t>Informationen und Link Corel Edustore</t>
+  </si>
+  <si>
+    <t>Informationen zu Citavi, Kurse / Schulungen, Download-Links</t>
+  </si>
+  <si>
+    <t>Informationen zu SPSS Installation, Download-Links</t>
+  </si>
+  <si>
+    <t>Informationen zu Office 365</t>
+  </si>
+  <si>
+    <t>Info Softwarekatalog, Suchoption nach Software</t>
+  </si>
+  <si>
+    <t>aktuelle News über neue Software</t>
+  </si>
+  <si>
+    <t>ganzer SW-Katalog in alphabet. Sortierung</t>
+  </si>
+  <si>
+    <t>allg. Information zur Installation v. Software</t>
+  </si>
+  <si>
+    <t>Information zum Konzept, Zugang und Administration v. Kurssoftware</t>
+  </si>
+  <si>
+    <t>Erläuterung d. verschiedenen Lizenzarten</t>
+  </si>
+  <si>
+    <t>Info SW-Dokumentation</t>
+  </si>
+  <si>
+    <t>Anleitung zu Gimp</t>
+  </si>
+  <si>
+    <t>Anleitung zu Groupwise</t>
+  </si>
+  <si>
+    <t>Anleitung zu Microsoft Hyper-V</t>
+  </si>
+  <si>
+    <t>Anleitung zu Vmware Workstation</t>
+  </si>
+  <si>
+    <t>Anleitung zu Juniper VPN</t>
+  </si>
+  <si>
+    <t>Anleitung zu Oracle VirtualBox</t>
+  </si>
+  <si>
+    <t>Anleitung zu VMware Player</t>
+  </si>
+  <si>
+    <t>Auflistung von Apps für UR-Dienstleistungen und sonstigen Apps</t>
+  </si>
+  <si>
+    <t>externer Link (Linux der Uni R ReX)</t>
+  </si>
+  <si>
+    <t>Informationen zu Apple On Campus, Login zu Campus-Store</t>
+  </si>
+  <si>
+    <t>Angebot, Öffnungszeiten, Formulare, Ansprechpartner</t>
+  </si>
+  <si>
+    <t>PC Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Laptop Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Apple Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Drucker Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Monitor Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Scanner Angebot und Konfigurationsinfo</t>
+  </si>
+  <si>
+    <t>Details zum Lieferservice, Ansprechpartner</t>
+  </si>
+  <si>
+    <t>Infos zum Angebot, Ansprechpartner</t>
+  </si>
+  <si>
+    <t>Infos Geräteausleihe, Kontakt f. Sutierende / Bedienstete</t>
+  </si>
+  <si>
+    <t>Link zu Unterpunkt Geräte</t>
+  </si>
+  <si>
+    <t>persöhnliche Leihliste</t>
+  </si>
+  <si>
+    <t>Link zu Formular zur Schadensmeldung, Hinweis Rechner identifizieren</t>
+  </si>
+  <si>
+    <t>allg. Info, sutdienbegleitende IT-Ausbildung</t>
+  </si>
+  <si>
+    <t>Link zu IT-Services / CIP-Pools /Reservierung</t>
+  </si>
+  <si>
+    <t>Informationen und Ansprechpartner</t>
+  </si>
+  <si>
+    <t>Informationen zu GRIPS, FAQ, Ansprechpartner</t>
+  </si>
+  <si>
+    <t>Information, Angebot, Anmeldung, Ansprechpartner</t>
+  </si>
+  <si>
+    <t>Information und Kontaktdaten, Verlinkung zur Mediathek</t>
+  </si>
+  <si>
+    <t>Informationen zum Angebot, Auflistung des Kursangebots im aktullen Semster</t>
+  </si>
+  <si>
+    <t>Struktur, Pflichtbereich, Wahlbereich, Zertifikat</t>
+  </si>
+  <si>
+    <t>FlexNow, Umbuchung</t>
+  </si>
+  <si>
+    <t>Link zur Auflistung d. Angebotes, Anmeldung, Archiv, EDV-Ausbildung</t>
+  </si>
+  <si>
+    <t>Ansprechpartner Koordination, Kursleiter</t>
+  </si>
+  <si>
+    <t>Information, Screencasting, Filmen, Ton, Preise</t>
+  </si>
+  <si>
+    <t>Informationen zum Weiterbildungsangebot</t>
+  </si>
+  <si>
+    <t>Ankkündigung, Standort/Öffnungszeiten CIP-Pools, Support</t>
+  </si>
+  <si>
+    <t>Anzeige d. CIP-Pools auf Lageplan</t>
+  </si>
+  <si>
+    <t>Ausstattung Software d. Linux / Windows CIP-Pools</t>
+  </si>
+  <si>
+    <t>Ausstattung Hardware d. Linux / Windows CIP-Pools</t>
+  </si>
+  <si>
+    <t>Reservierungsmöglichkeit der einzelnen CIP-Pools</t>
+  </si>
+  <si>
+    <t>allgemeine Benutzerordnung für die CIP-Pools</t>
+  </si>
+  <si>
+    <t>Infos zu CIP-Pools mit Klassenraumsoftware</t>
+  </si>
+  <si>
+    <t>Information über verfügbare Dateidienste an der Uni R</t>
+  </si>
+  <si>
+    <t>Information zu verschiedenen Laufwerken, typisches Pfadmapping und NetWare Rights</t>
+  </si>
+  <si>
+    <t>Info Zugang ohne Novell Client  über Netstorage, WebDAV, FTP, SAMBA MyFiles</t>
+  </si>
+  <si>
+    <t>Anleitung Einrichten Remote-Zugängen über RAS und SSH</t>
+  </si>
+  <si>
+    <t>Verlinkung zu Web-VPN und VPN-Client</t>
+  </si>
+  <si>
+    <t>Anleitung Emailversand von großen Dateien</t>
+  </si>
+  <si>
+    <t>Dienste und Aufgaben des RZ bezüglich des Datennetzes</t>
+  </si>
+  <si>
+    <t>externer Link (Geräteregistrierung)</t>
+  </si>
+  <si>
+    <t>externer Link (Wohnheime)</t>
+  </si>
+  <si>
+    <t>externer Link (WLAN)</t>
+  </si>
+  <si>
+    <t>externer Link (Eduroam)</t>
+  </si>
+  <si>
+    <t>externer Link (Conference-Service)</t>
+  </si>
+  <si>
+    <t>externer Link (Public Key Infrastruktur)</t>
+  </si>
+  <si>
+    <t>VPN-Zugang</t>
+  </si>
+  <si>
+    <t>externer Link (SSL VPN)</t>
+  </si>
+  <si>
+    <t>Erklärung digitale Zertifikate, Import internes Zertifkat</t>
+  </si>
+  <si>
+    <t>Information zu Druckzentrum, Druck CIP-Pool, Druckerübersicht, Konto verwalten, Installtion, Webprint, Wertcoupons</t>
+  </si>
+  <si>
+    <t>Kontaktdaten, Ansprechpartner Druckzentrum</t>
+  </si>
+  <si>
+    <t>Anleitung zum Login d. Kontoerawaltung</t>
+  </si>
+  <si>
+    <t>Anleitung Druckerinstallation (lokal, Netzwerk, MacOS)</t>
+  </si>
+  <si>
+    <t>Informationen und Links zu Gropuwise, Spamquarantäne</t>
+  </si>
+  <si>
+    <t>Puremessage Information, FAQ</t>
+  </si>
+  <si>
+    <t>Information zu Spam und Sicherheit</t>
+  </si>
+  <si>
+    <t>Auflistung der Regeln zu Emails</t>
+  </si>
+  <si>
+    <t>Information zur Archivierung</t>
+  </si>
+  <si>
+    <t>Information zu Groupwise, Support, Mobiles Arbeiten, IMAP, Anleitungen, bekannte Probleme</t>
+  </si>
+  <si>
+    <t>Anleitung Faxen</t>
+  </si>
+  <si>
+    <t>Information zu "Formular-Lesen"</t>
+  </si>
+  <si>
+    <t>Link und Information zu Mediatthek, FAQs</t>
+  </si>
+  <si>
+    <t>Informationen zum Zeitserver</t>
   </si>
 </sst>
 </file>
@@ -1312,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="E150" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H172" sqref="H172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1824,7 @@
         <v>14</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3">
@@ -1443,7 +1851,7 @@
         <v>88</v>
       </c>
       <c r="L9" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1462,7 +1870,7 @@
         <v>89</v>
       </c>
       <c r="L10" s="28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1477,7 +1885,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -1496,7 +1904,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1515,7 +1923,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
@@ -1534,7 +1942,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -1553,7 +1961,7 @@
         <v>19</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
@@ -1572,7 +1980,7 @@
         <v>20</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
@@ -1591,7 +1999,7 @@
         <v>21</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
@@ -1629,7 +2037,7 @@
         <v>22</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3">
@@ -1655,7 +2063,7 @@
         <v>90</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,7 +2082,7 @@
         <v>91</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,7 +2097,7 @@
         <v>23</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="15">
@@ -1716,7 +2124,7 @@
         <v>92</v>
       </c>
       <c r="L23" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1735,7 +2143,7 @@
         <v>93</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1754,7 +2162,7 @@
         <v>25</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1773,7 +2181,7 @@
         <v>94</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,7 +2200,7 @@
         <v>95</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1807,7 +2215,7 @@
         <v>24</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -1825,7 +2233,9 @@
       <c r="G29" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="25"/>
+      <c r="H29" s="25" t="s">
+        <v>228</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="15">
         <v>3</v>
@@ -1850,7 +2260,9 @@
       <c r="K30" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="28"/>
+      <c r="L30" s="28" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="31" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10"/>
@@ -1867,7 +2279,9 @@
       <c r="K31" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="L31" s="28"/>
+      <c r="L31" s="28" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="32" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
@@ -1880,7 +2294,9 @@
       <c r="G32" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="25" t="s">
+        <v>231</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="15">
         <v>3</v>
@@ -1905,7 +2321,9 @@
       <c r="K33" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="L33" s="28"/>
+      <c r="L33" s="28" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="34" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
@@ -1922,7 +2340,9 @@
       <c r="K34" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="L34" s="28"/>
+      <c r="L34" s="28" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="35" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
@@ -1939,7 +2359,9 @@
       <c r="K35" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="L35" s="28"/>
+      <c r="L35" s="28" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="36" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
@@ -1956,7 +2378,9 @@
       <c r="K36" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="L36" s="28"/>
+      <c r="L36" s="28" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="37" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10"/>
@@ -1969,7 +2393,9 @@
       <c r="G37" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="25"/>
+      <c r="H37" s="25" t="s">
+        <v>236</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -1986,7 +2412,9 @@
       <c r="G38" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="25"/>
+      <c r="H38" s="25" t="s">
+        <v>237</v>
+      </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2003,7 +2431,9 @@
       <c r="G39" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="25"/>
+      <c r="H39" s="25" t="s">
+        <v>238</v>
+      </c>
       <c r="I39" s="3"/>
       <c r="J39" s="15">
         <v>3</v>
@@ -2028,7 +2458,9 @@
       <c r="K40" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L40" s="28"/>
+      <c r="L40" s="28" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="41" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
@@ -2045,7 +2477,9 @@
       <c r="K41" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="L41" s="28"/>
+      <c r="L41" s="28" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="42" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="10"/>
@@ -2062,7 +2496,9 @@
       <c r="K42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="L42" s="28"/>
+      <c r="L42" s="28" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="43" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
@@ -2075,7 +2511,9 @@
       <c r="G43" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="25"/>
+      <c r="H43" s="25" t="s">
+        <v>242</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2092,7 +2530,9 @@
       <c r="G44" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H44" s="25"/>
+      <c r="H44" s="25" t="s">
+        <v>243</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2109,7 +2549,9 @@
       <c r="G45" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="H45" s="25"/>
+      <c r="H45" s="25" t="s">
+        <v>244</v>
+      </c>
       <c r="I45" s="3"/>
       <c r="J45" s="15">
         <v>3</v>
@@ -2134,7 +2576,9 @@
       <c r="K46" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L46" s="28"/>
+      <c r="L46" s="28" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="47" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
@@ -2151,7 +2595,9 @@
       <c r="K47" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="L47" s="28"/>
+      <c r="L47" s="28" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="48" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
@@ -2168,7 +2614,9 @@
       <c r="K48" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="L48" s="28"/>
+      <c r="L48" s="28" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="49" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="10"/>
@@ -2185,7 +2633,9 @@
       <c r="K49" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="L49" s="28"/>
+      <c r="L49" s="28" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="50" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="10"/>
@@ -2198,7 +2648,9 @@
       <c r="G50" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H50" s="25"/>
+      <c r="H50" s="25" t="s">
+        <v>249</v>
+      </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2215,7 +2667,9 @@
       <c r="G51" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H51" s="25"/>
+      <c r="H51" s="25" t="s">
+        <v>250</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3">
         <v>3</v>
@@ -2240,7 +2694,9 @@
       <c r="K52" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="L52" s="28"/>
+      <c r="L52" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="53" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="10"/>
@@ -2257,7 +2713,9 @@
       <c r="K53" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="L53" s="28"/>
+      <c r="L53" s="28" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="54" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="10"/>
@@ -2274,7 +2732,9 @@
       <c r="K54" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="L54" s="28"/>
+      <c r="L54" s="28" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="55" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="10"/>
@@ -2287,7 +2747,9 @@
       <c r="G55" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="25"/>
+      <c r="H55" s="25" t="s">
+        <v>254</v>
+      </c>
       <c r="I55" s="3"/>
       <c r="J55" s="15">
         <v>3</v>
@@ -2312,7 +2774,9 @@
       <c r="K56" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="L56" s="28"/>
+      <c r="L56" s="28" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="57" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="10"/>
@@ -2329,7 +2793,9 @@
       <c r="K57" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="L57" s="28"/>
+      <c r="L57" s="28" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="58" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="10"/>
@@ -2346,7 +2812,9 @@
       <c r="K58" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="L58" s="28"/>
+      <c r="L58" s="28" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="59" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="10"/>
@@ -2359,7 +2827,9 @@
       <c r="G59" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H59" s="25"/>
+      <c r="H59" s="25" t="s">
+        <v>258</v>
+      </c>
       <c r="I59" s="3"/>
       <c r="J59" s="15">
         <v>3</v>
@@ -2384,7 +2854,9 @@
       <c r="K60" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="L60" s="28"/>
+      <c r="L60" s="28" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="61" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="10"/>
@@ -2401,7 +2873,9 @@
       <c r="K61" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="L61" s="28"/>
+      <c r="L61" s="28" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="62" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="10"/>
@@ -2418,7 +2892,9 @@
       <c r="K62" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L62" s="28"/>
+      <c r="L62" s="28" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="63" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="10"/>
@@ -2431,7 +2907,9 @@
       <c r="G63" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H63" s="25"/>
+      <c r="H63" s="25" t="s">
+        <v>262</v>
+      </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3">
         <v>3</v>
@@ -2456,7 +2934,9 @@
       <c r="K64" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="L64" s="28"/>
+      <c r="L64" s="28" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="65" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="10"/>
@@ -2473,7 +2953,9 @@
       <c r="K65" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="L65" s="28"/>
+      <c r="L65" s="28" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="66" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="10"/>
@@ -2490,7 +2972,9 @@
       <c r="K66" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="L66" s="28"/>
+      <c r="L66" s="28" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="67" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="10"/>
@@ -2507,7 +2991,9 @@
       <c r="K67" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="L67" s="28"/>
+      <c r="L67" s="28" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="68" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10"/>
@@ -2524,7 +3010,9 @@
       <c r="K68" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="L68" s="28"/>
+      <c r="L68" s="28" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="69" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10"/>
@@ -2541,7 +3029,9 @@
       <c r="K69" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="L69" s="28"/>
+      <c r="L69" s="28" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="70" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="10"/>
@@ -2558,7 +3048,9 @@
       <c r="K70" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="L70" s="28"/>
+      <c r="L70" s="28" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="71" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="10"/>
@@ -2571,7 +3063,9 @@
       <c r="G71" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H71" s="25"/>
+      <c r="H71" s="25" t="s">
+        <v>266</v>
+      </c>
       <c r="I71" s="3"/>
       <c r="J71" s="15">
         <v>3</v>
@@ -2596,7 +3090,9 @@
       <c r="K72" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="L72" s="28"/>
+      <c r="L72" s="28" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="73" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="12">
@@ -2628,7 +3124,9 @@
       <c r="G74" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H74" s="25"/>
+      <c r="H74" s="25" t="s">
+        <v>268</v>
+      </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -2645,7 +3143,9 @@
       <c r="G75" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H75" s="25"/>
+      <c r="H75" s="25" t="s">
+        <v>269</v>
+      </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -2662,7 +3162,9 @@
       <c r="G76" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H76" s="25"/>
+      <c r="H76" s="25" t="s">
+        <v>270</v>
+      </c>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -2679,7 +3181,9 @@
       <c r="G77" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H77" s="25"/>
+      <c r="H77" s="25" t="s">
+        <v>271</v>
+      </c>
       <c r="I77" s="3"/>
       <c r="J77" s="15">
         <v>3</v>
@@ -2704,7 +3208,9 @@
       <c r="K78" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="L78" s="28"/>
+      <c r="L78" s="28" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="79" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10"/>
@@ -2721,7 +3227,9 @@
       <c r="K79" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="L79" s="28"/>
+      <c r="L79" s="28" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="80" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="10"/>
@@ -2738,7 +3246,9 @@
       <c r="K80" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L80" s="28"/>
+      <c r="L80" s="28" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="81" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10"/>
@@ -2755,7 +3265,9 @@
       <c r="K81" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="L81" s="28"/>
+      <c r="L81" s="28" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="82" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="10"/>
@@ -2772,7 +3284,9 @@
       <c r="K82" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L82" s="28"/>
+      <c r="L82" s="28" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="83" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="10"/>
@@ -2789,7 +3303,9 @@
       <c r="K83" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="L83" s="28"/>
+      <c r="L83" s="28" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="84" spans="2:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="10"/>
@@ -2806,7 +3322,9 @@
       <c r="K84" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="L84" s="28"/>
+      <c r="L84" s="28" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="85" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="10"/>
@@ -2819,7 +3337,9 @@
       <c r="G85" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H85" s="25"/>
+      <c r="H85" s="25" t="s">
+        <v>279</v>
+      </c>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -2836,7 +3356,9 @@
       <c r="G86" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H86" s="25"/>
+      <c r="H86" s="25" t="s">
+        <v>280</v>
+      </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3">
         <v>3</v>
@@ -2861,7 +3383,9 @@
       <c r="K87" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="L87" s="28"/>
+      <c r="L87" s="28" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="88" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="10"/>
@@ -2878,7 +3402,9 @@
       <c r="K88" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="L88" s="28"/>
+      <c r="L88" s="28" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="89" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="10"/>
@@ -2895,7 +3421,9 @@
       <c r="K89" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="L89" s="28"/>
+      <c r="L89" s="28" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="90" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="10"/>
@@ -2912,7 +3440,9 @@
       <c r="K90" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="L90" s="28"/>
+      <c r="L90" s="28" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="91" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="10"/>
@@ -2925,7 +3455,9 @@
       <c r="G91" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H91" s="25"/>
+      <c r="H91" s="25" t="s">
+        <v>285</v>
+      </c>
       <c r="I91" s="3"/>
       <c r="J91" s="3">
         <v>3</v>
@@ -2950,7 +3482,9 @@
       <c r="K92" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="L92" s="28"/>
+      <c r="L92" s="28" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="93" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="10"/>
@@ -2967,7 +3501,9 @@
       <c r="K93" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="L93" s="28"/>
+      <c r="L93" s="28" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="94" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="10"/>
@@ -2984,7 +3520,9 @@
       <c r="K94" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="L94" s="28"/>
+      <c r="L94" s="28" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="95" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="10"/>
@@ -3001,7 +3539,9 @@
       <c r="K95" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="L95" s="28"/>
+      <c r="L95" s="28" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="96" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="10"/>
@@ -3018,7 +3558,9 @@
       <c r="K96" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="L96" s="28"/>
+      <c r="L96" s="28" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="97" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="10"/>
@@ -3031,7 +3573,9 @@
       <c r="G97" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H97" s="25"/>
+      <c r="H97" s="25" t="s">
+        <v>291</v>
+      </c>
       <c r="I97" s="3"/>
       <c r="J97" s="3">
         <v>3</v>
@@ -3056,7 +3600,9 @@
       <c r="K98" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="L98" s="28"/>
+      <c r="L98" s="28" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="99" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="10"/>
@@ -3073,7 +3619,9 @@
       <c r="K99" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="L99" s="28"/>
+      <c r="L99" s="28" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="100" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="10"/>
@@ -3090,7 +3638,9 @@
       <c r="K100" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L100" s="28"/>
+      <c r="L100" s="28" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="101" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="10"/>
@@ -3107,7 +3657,9 @@
       <c r="K101" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="L101" s="28"/>
+      <c r="L101" s="28" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="102" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="10"/>
@@ -3124,7 +3676,9 @@
       <c r="K102" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="L102" s="28"/>
+      <c r="L102" s="28" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="103" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="10"/>
@@ -3141,7 +3695,9 @@
       <c r="K103" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="L103" s="28"/>
+      <c r="L103" s="28" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="104" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="10"/>
@@ -3158,7 +3714,9 @@
       <c r="K104" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L104" s="28"/>
+      <c r="L104" s="28" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="105" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="10"/>
@@ -3171,7 +3729,9 @@
       <c r="G105" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H105" s="25"/>
+      <c r="H105" s="25" t="s">
+        <v>299</v>
+      </c>
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
@@ -3188,7 +3748,9 @@
       <c r="G106" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H106" s="25"/>
+      <c r="H106" s="25" t="s">
+        <v>300</v>
+      </c>
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
@@ -3224,7 +3786,9 @@
       <c r="G108" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H108" s="25"/>
+      <c r="H108" s="25" t="s">
+        <v>301</v>
+      </c>
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
@@ -3241,7 +3805,9 @@
       <c r="G109" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="H109" s="25"/>
+      <c r="H109" s="25" t="s">
+        <v>302</v>
+      </c>
       <c r="I109" s="3"/>
       <c r="J109" s="3">
         <v>3</v>
@@ -3266,7 +3832,9 @@
       <c r="K110" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="L110" s="28"/>
+      <c r="L110" s="28" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="111" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="10"/>
@@ -3283,7 +3851,9 @@
       <c r="K111" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="L111" s="28"/>
+      <c r="L111" s="28" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="112" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="10"/>
@@ -3300,7 +3870,9 @@
       <c r="K112" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="L112" s="28"/>
+      <c r="L112" s="28" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="113" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="10"/>
@@ -3317,7 +3889,9 @@
       <c r="K113" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="L113" s="28"/>
+      <c r="L113" s="28" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="114" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="10"/>
@@ -3334,7 +3908,9 @@
       <c r="K114" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="L114" s="28"/>
+      <c r="L114" s="28" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="115" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="10"/>
@@ -3351,7 +3927,9 @@
       <c r="K115" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="L115" s="28"/>
+      <c r="L115" s="28" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="116" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="10"/>
@@ -3364,7 +3942,9 @@
       <c r="G116" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H116" s="25"/>
+      <c r="H116" s="25" t="s">
+        <v>309</v>
+      </c>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
@@ -3381,7 +3961,9 @@
       <c r="G117" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H117" s="25"/>
+      <c r="H117" s="25" t="s">
+        <v>310</v>
+      </c>
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
@@ -3398,7 +3980,9 @@
       <c r="G118" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H118" s="25"/>
+      <c r="H118" s="25" t="s">
+        <v>312</v>
+      </c>
       <c r="I118" s="3"/>
       <c r="J118" s="3">
         <v>3</v>
@@ -3423,7 +4007,9 @@
       <c r="K119" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="L119" s="28"/>
+      <c r="L119" s="28" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="120" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="10"/>
@@ -3440,7 +4026,9 @@
       <c r="K120" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="L120" s="28"/>
+      <c r="L120" s="28" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="121" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="10"/>
@@ -3453,7 +4041,9 @@
       <c r="G121" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H121" s="25"/>
+      <c r="H121" s="25" t="s">
+        <v>314</v>
+      </c>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
@@ -3467,7 +4057,7 @@
         <v>9</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>205</v>
+        <v>315</v>
       </c>
       <c r="E122" s="12"/>
       <c r="F122" s="3"/>
@@ -3489,7 +4079,9 @@
       <c r="G123" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H123" s="25"/>
+      <c r="H123" s="25" t="s">
+        <v>316</v>
+      </c>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
@@ -3506,7 +4098,9 @@
       <c r="G124" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H124" s="25"/>
+      <c r="H124" s="25" t="s">
+        <v>317</v>
+      </c>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
@@ -3523,7 +4117,9 @@
       <c r="G125" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="H125" s="25"/>
+      <c r="H125" s="25" t="s">
+        <v>318</v>
+      </c>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
@@ -3540,7 +4136,9 @@
       <c r="G126" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H126" s="25"/>
+      <c r="H126" s="25" t="s">
+        <v>319</v>
+      </c>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
@@ -3557,7 +4155,9 @@
       <c r="G127" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H127" s="25"/>
+      <c r="H127" s="25" t="s">
+        <v>320</v>
+      </c>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
@@ -3574,7 +4174,9 @@
       <c r="G128" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H128" s="25"/>
+      <c r="H128" s="25" t="s">
+        <v>321</v>
+      </c>
       <c r="I128" s="3"/>
       <c r="J128" s="3">
         <v>3</v>
@@ -3599,7 +4201,9 @@
       <c r="K129" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="L129" s="28"/>
+      <c r="L129" s="28" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="130" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="10"/>
@@ -3616,7 +4220,9 @@
       <c r="K130" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L130" s="28"/>
+      <c r="L130" s="28" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="131" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="10"/>
@@ -3633,7 +4239,9 @@
       <c r="K131" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="L131" s="28"/>
+      <c r="L131" s="28" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="132" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="10"/>
@@ -3650,7 +4258,9 @@
       <c r="K132" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="L132" s="28"/>
+      <c r="L132" s="28" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="133" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="10"/>
@@ -3663,7 +4273,9 @@
       <c r="G133" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H133" s="25"/>
+      <c r="H133" s="25" t="s">
+        <v>326</v>
+      </c>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
@@ -3680,7 +4292,9 @@
       <c r="G134" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="H134" s="25"/>
+      <c r="H134" s="25" t="s">
+        <v>327</v>
+      </c>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
@@ -3694,7 +4308,7 @@
         <v>10</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E135" s="12"/>
       <c r="F135" s="3"/>
@@ -3716,7 +4330,9 @@
       <c r="G136" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="H136" s="25"/>
+      <c r="H136" s="25" t="s">
+        <v>328</v>
+      </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3">
         <v>3</v>
@@ -3741,7 +4357,9 @@
       <c r="K137" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L137" s="28"/>
+      <c r="L137" s="28" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="138" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="10"/>
@@ -3758,7 +4376,9 @@
       <c r="K138" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L138" s="28"/>
+      <c r="L138" s="28" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="139" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="10"/>
@@ -3775,7 +4395,9 @@
       <c r="K139" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="L139" s="28"/>
+      <c r="L139" s="28" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="140" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="10"/>
@@ -3792,7 +4414,9 @@
       <c r="K140" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="L140" s="28"/>
+      <c r="L140" s="28" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="141" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="10"/>
@@ -3809,7 +4433,9 @@
       <c r="K141" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="L141" s="28"/>
+      <c r="L141" s="28" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="142" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="10"/>
@@ -3826,7 +4452,9 @@
       <c r="K142" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="L142" s="28"/>
+      <c r="L142" s="28" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="143" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="10"/>
@@ -3839,7 +4467,9 @@
       <c r="G143" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H143" s="25"/>
+      <c r="H143" s="25" t="s">
+        <v>335</v>
+      </c>
       <c r="I143" s="3"/>
       <c r="J143" s="3">
         <v>3</v>
@@ -3864,7 +4494,9 @@
       <c r="K144" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="L144" s="28"/>
+      <c r="L144" s="28" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="145" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="10"/>
@@ -3881,7 +4513,9 @@
       <c r="K145" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="L145" s="28"/>
+      <c r="L145" s="28" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="146" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="10"/>
@@ -3898,7 +4532,9 @@
       <c r="K146" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="L146" s="28"/>
+      <c r="L146" s="28" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="147" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="10"/>
@@ -3915,7 +4551,9 @@
       <c r="K147" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L147" s="28"/>
+      <c r="L147" s="28" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="148" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="10"/>
@@ -3932,7 +4570,9 @@
       <c r="K148" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="L148" s="28"/>
+      <c r="L148" s="28" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="149" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="10"/>
@@ -3945,7 +4585,9 @@
       <c r="G149" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H149" s="25"/>
+      <c r="H149" s="25" t="s">
+        <v>341</v>
+      </c>
       <c r="I149" s="3"/>
       <c r="J149" s="3">
         <v>3</v>
@@ -3970,7 +4612,9 @@
       <c r="K150" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="L150" s="28"/>
+      <c r="L150" s="28" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="151" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="10"/>
@@ -3987,7 +4631,9 @@
       <c r="K151" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="L151" s="28"/>
+      <c r="L151" s="28" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="152" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="10"/>
@@ -4004,7 +4650,9 @@
       <c r="K152" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L152" s="28"/>
+      <c r="L152" s="28" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="153" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="10"/>
@@ -4021,7 +4669,9 @@
       <c r="K153" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="L153" s="28"/>
+      <c r="L153" s="28" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="154" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="10"/>
@@ -4038,7 +4688,9 @@
       <c r="K154" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="L154" s="28"/>
+      <c r="L154" s="28" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="155" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="10"/>
@@ -4055,7 +4707,9 @@
       <c r="K155" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="L155" s="28"/>
+      <c r="L155" s="28" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="156" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="10"/>
@@ -4069,8 +4723,12 @@
       <c r="J156" s="16">
         <v>3</v>
       </c>
-      <c r="K156" s="11"/>
-      <c r="L156" s="28"/>
+      <c r="K156" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="L156" s="28" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="157" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="10"/>
@@ -4083,7 +4741,9 @@
       <c r="G157" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H157" s="25"/>
+      <c r="H157" s="25" t="s">
+        <v>350</v>
+      </c>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
@@ -4100,7 +4760,9 @@
       <c r="G158" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H158" s="25"/>
+      <c r="H158" s="25" t="s">
+        <v>351</v>
+      </c>
       <c r="I158" s="3"/>
       <c r="J158" s="3">
         <v>3</v>
@@ -4125,7 +4787,9 @@
       <c r="K159" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="L159" s="28"/>
+      <c r="L159" s="28" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="160" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10"/>
@@ -4142,7 +4806,9 @@
       <c r="K160" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="L160" s="28"/>
+      <c r="L160" s="28" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="161" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="10"/>
@@ -4159,7 +4825,9 @@
       <c r="K161" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="L161" s="28"/>
+      <c r="L161" s="28" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="162" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="10"/>
@@ -4172,7 +4840,9 @@
       <c r="G162" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H162" s="25"/>
+      <c r="H162" s="25" t="s">
+        <v>355</v>
+      </c>
       <c r="I162" s="3"/>
       <c r="J162" s="3">
         <v>3</v>
@@ -4197,7 +4867,9 @@
       <c r="K163" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="L163" s="28"/>
+      <c r="L163" s="28" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="164" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="10"/>
@@ -4214,7 +4886,9 @@
       <c r="K164" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="L164" s="28"/>
+      <c r="L164" s="28" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="165" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="10"/>
@@ -4231,7 +4905,9 @@
       <c r="K165" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="L165" s="28"/>
+      <c r="L165" s="28" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="166" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="10"/>
@@ -4248,7 +4924,9 @@
       <c r="K166" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="L166" s="28"/>
+      <c r="L166" s="28" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="167" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="10"/>
@@ -4261,7 +4939,9 @@
       <c r="G167" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H167" s="25"/>
+      <c r="H167" s="25" t="s">
+        <v>360</v>
+      </c>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
@@ -4278,7 +4958,9 @@
       <c r="G168" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="H168" s="25"/>
+      <c r="H168" s="25" t="s">
+        <v>361</v>
+      </c>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
@@ -4295,7 +4977,9 @@
       <c r="G169" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H169" s="25"/>
+      <c r="H169" s="25" t="s">
+        <v>362</v>
+      </c>
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
@@ -4312,7 +4996,9 @@
       <c r="G170" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="H170" s="25"/>
+      <c r="H170" s="25" t="s">
+        <v>363</v>
+      </c>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
@@ -4329,7 +5015,9 @@
       <c r="G171" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H171" s="25"/>
+      <c r="H171" s="25" t="s">
+        <v>364</v>
+      </c>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
@@ -4699,7 +5387,7 @@
         <v>11</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E192" s="12"/>
       <c r="F192" s="3"/>
@@ -4926,7 +5614,7 @@
         <v>12</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E205" s="10"/>
       <c r="F205" s="16"/>

</xml_diff>

<commit_message>
Fertigstellung d. Content Analyse
</commit_message>
<xml_diff>
--- a/Content Analyse.xlsx
+++ b/Content Analyse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="398">
   <si>
     <t>Content Analyse RZ-Webseite</t>
   </si>
@@ -1119,6 +1119,105 @@
   </si>
   <si>
     <t>Informationen zum Zeitserver</t>
+  </si>
+  <si>
+    <t>Literatur, Antragsformular und Links zu High Performance Computing</t>
+  </si>
+  <si>
+    <t>Information, Kontaktdaten, personalisierte SW-Lösung</t>
+  </si>
+  <si>
+    <t>spezielle Information zu EVO und Panda, Links</t>
+  </si>
+  <si>
+    <t>Sophos, Installation, Aktualisierung und Konfiguration von Virenscanner</t>
+  </si>
+  <si>
+    <t>Information zu Virtualisierung, Produktübersicht, Anforderungen., Vorteile, Datenaustausch, Installation</t>
+  </si>
+  <si>
+    <t>Kontaktdaten, Schwarzes Brett, Zugang Webserver, Dokumentation</t>
+  </si>
+  <si>
+    <t>allg. Nutzungsbedingungen für private Homepages</t>
+  </si>
+  <si>
+    <t>FAQs</t>
+  </si>
+  <si>
+    <t>Antrag eigene Homepage, Zugangsmethoden</t>
+  </si>
+  <si>
+    <t>versch. Information zu persönlicher Homepage</t>
+  </si>
+  <si>
+    <t>Zugangsmethoden zur eigenen Homepage</t>
+  </si>
+  <si>
+    <t>Information, Antrag auf Zugang, Anleitung Samba / Linux, Zugriffssteuerung</t>
+  </si>
+  <si>
+    <t>Hilfestellung: Dateinamen Konvention</t>
+  </si>
+  <si>
+    <t>Anleitung automatisierte Windows-Installation</t>
+  </si>
+  <si>
+    <t>externer Link (RZ-Windows-Update-Service)</t>
+  </si>
+  <si>
+    <t>ReX-Linux d. Uni R, Allgemeine Information</t>
+  </si>
+  <si>
+    <t>Installationsanleitung, Partitionierung</t>
+  </si>
+  <si>
+    <t>Administrationsanleitung</t>
+  </si>
+  <si>
+    <t>leere Seite</t>
+  </si>
+  <si>
+    <t>Download TSM-Client</t>
+  </si>
+  <si>
+    <t>Kontaktdaten</t>
+  </si>
+  <si>
+    <t>allgemeine Information zu Ausbildungsstellen und Kontaktdaten</t>
+  </si>
+  <si>
+    <t>Informationen Azubi-Camp</t>
+  </si>
+  <si>
+    <t>Aufgaben d. Azubis</t>
+  </si>
+  <si>
+    <t>Auflistung aller Mitarbeiter und Kontaktdaten</t>
+  </si>
+  <si>
+    <t>Anfahrtgsbeschreibung, Gebäudepläne</t>
+  </si>
+  <si>
+    <t>aktuelle Stellenausschribung, Kontaktdaten, Arbeits-/Entgeltbedingungen</t>
+  </si>
+  <si>
+    <t>Anmeldung zum Newsletter (RZettel)</t>
+  </si>
+  <si>
+    <t>grafische Darstellung d. Organisation, Auflistung der Abteilungen</t>
+  </si>
+  <si>
+    <t>Liste der Jahresberichte</t>
+  </si>
+  <si>
+    <t>Berichte Studienbeiträge zu bestimmten Themen</t>
+  </si>
+  <si>
+    <t>Benutzerordnungen, Datenschutz/-sicherheit,</t>
+  </si>
+  <si>
+    <t>Login zur Literaturansicht</t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1436,6 +1535,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1720,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E150" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H172" sqref="H172"/>
+    <sheetView tabSelected="1" topLeftCell="E162" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J178" sqref="J178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5034,7 +5136,9 @@
       <c r="G172" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H172" s="25"/>
+      <c r="H172" s="25" t="s">
+        <v>365</v>
+      </c>
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
@@ -5051,7 +5155,9 @@
       <c r="G173" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H173" s="25"/>
+      <c r="H173" s="25" t="s">
+        <v>366</v>
+      </c>
       <c r="I173" s="3"/>
       <c r="J173" s="3">
         <v>3</v>
@@ -5076,7 +5182,9 @@
       <c r="K174" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="L174" s="28"/>
+      <c r="L174" s="28" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="175" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="10"/>
@@ -5089,7 +5197,9 @@
       <c r="G175" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="H175" s="25"/>
+      <c r="H175" s="25" t="s">
+        <v>368</v>
+      </c>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -5106,7 +5216,9 @@
       <c r="G176" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H176" s="25"/>
+      <c r="H176" s="25" t="s">
+        <v>369</v>
+      </c>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
@@ -5123,7 +5235,9 @@
       <c r="G177" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H177" s="25"/>
+      <c r="H177" s="25" t="s">
+        <v>370</v>
+      </c>
       <c r="I177" s="3"/>
       <c r="J177" s="3">
         <v>3</v>
@@ -5148,7 +5262,9 @@
       <c r="K178" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="L178" s="28"/>
+      <c r="L178" s="28" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="179" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="10"/>
@@ -5165,7 +5281,9 @@
       <c r="K179" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="L179" s="28"/>
+      <c r="L179" s="28" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="180" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="10"/>
@@ -5182,7 +5300,9 @@
       <c r="K180" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="L180" s="28"/>
+      <c r="L180" s="28" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="181" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="10"/>
@@ -5199,7 +5319,9 @@
       <c r="K181" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="L181" s="28"/>
+      <c r="L181" s="28" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="182" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="10"/>
@@ -5216,7 +5338,9 @@
       <c r="K182" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="L182" s="28"/>
+      <c r="L182" s="28" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="183" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="10"/>
@@ -5233,7 +5357,9 @@
       <c r="K183" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="L183" s="28"/>
+      <c r="L183" s="28" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="184" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="10"/>
@@ -5250,7 +5376,9 @@
       <c r="K184" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="L184" s="28"/>
+      <c r="L184" s="28" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="185" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="10"/>
@@ -5263,7 +5391,9 @@
       <c r="G185" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="H185" s="25"/>
+      <c r="H185" s="25" t="s">
+        <v>378</v>
+      </c>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
@@ -5280,7 +5410,9 @@
       <c r="G186" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="H186" s="25"/>
+      <c r="H186" s="25" t="s">
+        <v>379</v>
+      </c>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
@@ -5297,7 +5429,9 @@
       <c r="G187" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="H187" s="25"/>
+      <c r="H187" s="25" t="s">
+        <v>380</v>
+      </c>
       <c r="I187" s="3"/>
       <c r="J187" s="3">
         <v>3</v>
@@ -5322,7 +5456,9 @@
       <c r="K188" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="L188" s="28"/>
+      <c r="L188" s="28" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="189" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="10"/>
@@ -5339,7 +5475,9 @@
       <c r="K189" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="L189" s="28"/>
+      <c r="L189" s="28" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="190" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="10"/>
@@ -5352,7 +5490,9 @@
       <c r="G190" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="H190" s="25"/>
+      <c r="H190" s="25" t="s">
+        <v>383</v>
+      </c>
       <c r="I190" s="3"/>
       <c r="J190" s="15">
         <v>3</v>
@@ -5377,7 +5517,9 @@
       <c r="K191" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="L191" s="28"/>
+      <c r="L191" s="28" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="192" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="12">
@@ -5409,7 +5551,9 @@
       <c r="G193" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H193" s="25"/>
+      <c r="H193" s="25" t="s">
+        <v>385</v>
+      </c>
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3"/>
@@ -5426,7 +5570,9 @@
       <c r="G194" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H194" s="25"/>
+      <c r="H194" s="25" t="s">
+        <v>386</v>
+      </c>
       <c r="I194" s="3"/>
       <c r="J194" s="3">
         <v>3</v>
@@ -5451,7 +5597,9 @@
       <c r="K195" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="L195" s="28"/>
+      <c r="L195" s="28" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="196" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10"/>
@@ -5468,7 +5616,9 @@
       <c r="K196" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="L196" s="28"/>
+      <c r="L196" s="28" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="197" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10"/>
@@ -5481,7 +5631,9 @@
       <c r="G197" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="H197" s="30"/>
+      <c r="H197" s="30" t="s">
+        <v>389</v>
+      </c>
       <c r="I197" s="20"/>
       <c r="J197" s="20"/>
       <c r="K197" s="20"/>
@@ -5498,7 +5650,9 @@
       <c r="G198" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="H198" s="30"/>
+      <c r="H198" s="30" t="s">
+        <v>390</v>
+      </c>
       <c r="I198" s="20"/>
       <c r="J198" s="20"/>
       <c r="K198" s="20"/>
@@ -5515,7 +5669,9 @@
       <c r="G199" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="H199" s="30"/>
+      <c r="H199" s="30" t="s">
+        <v>391</v>
+      </c>
       <c r="I199" s="20"/>
       <c r="J199" s="20"/>
       <c r="K199" s="20"/>
@@ -5532,7 +5688,9 @@
       <c r="G200" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H200" s="30"/>
+      <c r="H200" s="30" t="s">
+        <v>392</v>
+      </c>
       <c r="I200" s="20"/>
       <c r="J200" s="20"/>
       <c r="K200" s="20"/>
@@ -5549,7 +5707,9 @@
       <c r="G201" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="H201" s="30"/>
+      <c r="H201" s="30" t="s">
+        <v>393</v>
+      </c>
       <c r="I201" s="20"/>
       <c r="J201" s="20"/>
       <c r="K201" s="20"/>
@@ -5566,7 +5726,9 @@
       <c r="G202" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H202" s="30"/>
+      <c r="H202" s="30" t="s">
+        <v>394</v>
+      </c>
       <c r="I202" s="20"/>
       <c r="J202" s="20"/>
       <c r="K202" s="20"/>
@@ -5580,10 +5742,12 @@
       <c r="F203" s="19">
         <v>2</v>
       </c>
-      <c r="G203" s="19" t="s">
+      <c r="G203" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="H203" s="30"/>
+      <c r="H203" s="30" t="s">
+        <v>395</v>
+      </c>
       <c r="I203" s="20"/>
       <c r="J203" s="20"/>
       <c r="K203" s="20"/>
@@ -5600,7 +5764,9 @@
       <c r="G204" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="H204" s="30"/>
+      <c r="H204" s="30" t="s">
+        <v>396</v>
+      </c>
       <c r="I204" s="20"/>
       <c r="J204" s="20"/>
       <c r="K204" s="20"/>
@@ -5636,7 +5802,9 @@
       <c r="G206" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H206" s="25"/>
+      <c r="H206" s="25" t="s">
+        <v>397</v>
+      </c>
       <c r="I206" s="3"/>
       <c r="J206" s="3">
         <v>3</v>

</xml_diff>